<commit_message>
Pre outcome measures updated
</commit_message>
<xml_diff>
--- a/data/GOZO_brief_parent.xlsx
+++ b/data/GOZO_brief_parent.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/KAHI/participant_1_data/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/GOZO/participant_3_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94FBE3B-4C43-434A-B4EB-24B9B369845E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D23E23-BB75-CF47-B2E4-B6528516B82C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="1060" windowWidth="26840" windowHeight="14760" xr2:uid="{061739A5-0582-EE47-A472-C84BB2AE7FED}"/>
   </bookViews>
@@ -90,7 +90,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -441,7 +441,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.83203125" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
@@ -449,7 +449,7 @@
     <col min="4" max="4" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,108 +463,108 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pre treatment phase outcome measurements added
</commit_message>
<xml_diff>
--- a/data/GOZO_brief_parent.xlsx
+++ b/data/GOZO_brief_parent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/GOZO/participant_3_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448CB1AF-4AEB-674B-9981-CE3EA619FF7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BA1BC8-DC2C-CB4B-8613-B43AB44675F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="1060" windowWidth="26840" windowHeight="14760" xr2:uid="{061739A5-0582-EE47-A472-C84BB2AE7FED}"/>
+    <workbookView xWindow="38640" yWindow="5900" windowWidth="26840" windowHeight="14760" xr2:uid="{061739A5-0582-EE47-A472-C84BB2AE7FED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,16 +74,16 @@
     <t>Plan/Organize Scale</t>
   </si>
   <si>
-    <t>Organization Scale</t>
-  </si>
-  <si>
     <t>Cognitive Regulation Index</t>
   </si>
   <si>
     <t xml:space="preserve">Global Executive Composite </t>
   </si>
   <si>
-    <t>Task Completion Scale</t>
+    <t>Task-Monitor Scale</t>
+  </si>
+  <si>
+    <t>Organization of Materials Scale</t>
   </si>
 </sst>
 </file>
@@ -438,12 +438,12 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="20.83203125" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" customWidth="1"/>
@@ -470,6 +470,9 @@
       <c r="B2">
         <v>68</v>
       </c>
+      <c r="C2">
+        <v>62</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -478,6 +481,9 @@
       <c r="B3">
         <v>70</v>
       </c>
+      <c r="C3">
+        <v>65</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -486,6 +492,9 @@
       <c r="B4">
         <v>71</v>
       </c>
+      <c r="C4">
+        <v>64</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -494,6 +503,9 @@
       <c r="B5">
         <v>72</v>
       </c>
+      <c r="C5">
+        <v>68</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -502,6 +514,9 @@
       <c r="B6">
         <v>83</v>
       </c>
+      <c r="C6">
+        <v>62</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -510,6 +525,9 @@
       <c r="B7">
         <v>82</v>
       </c>
+      <c r="C7">
+        <v>66</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -518,6 +536,9 @@
       <c r="B8">
         <v>70</v>
       </c>
+      <c r="C8">
+        <v>70</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -526,6 +547,9 @@
       <c r="B9">
         <v>72</v>
       </c>
+      <c r="C9">
+        <v>70</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -534,37 +558,52 @@
       <c r="B10">
         <v>71</v>
       </c>
+      <c r="C10">
+        <v>58</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>47</v>
       </c>
+      <c r="C11">
+        <v>61</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>53</v>
       </c>
+      <c r="C12">
+        <v>49</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>66</v>
       </c>
+      <c r="C13">
+        <v>64</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>72</v>
+      </c>
+      <c r="C14">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final parent outcome measures added
</commit_message>
<xml_diff>
--- a/data/GOZO_brief_parent.xlsx
+++ b/data/GOZO_brief_parent.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/GOZO/participant_3_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BA1BC8-DC2C-CB4B-8613-B43AB44675F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174E9C26-501C-AE4A-929A-8893FAC36611}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38640" yWindow="5900" windowWidth="26840" windowHeight="14760" xr2:uid="{061739A5-0582-EE47-A472-C84BB2AE7FED}"/>
   </bookViews>
@@ -438,7 +438,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -473,6 +473,9 @@
       <c r="C2">
         <v>62</v>
       </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -484,6 +487,9 @@
       <c r="C3">
         <v>65</v>
       </c>
+      <c r="D3">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -495,6 +501,9 @@
       <c r="C4">
         <v>64</v>
       </c>
+      <c r="D4">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -506,6 +515,9 @@
       <c r="C5">
         <v>68</v>
       </c>
+      <c r="D5">
+        <v>65</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -517,6 +529,9 @@
       <c r="C6">
         <v>62</v>
       </c>
+      <c r="D6">
+        <v>48</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -528,6 +543,9 @@
       <c r="C7">
         <v>66</v>
       </c>
+      <c r="D7">
+        <v>56</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -539,6 +557,9 @@
       <c r="C8">
         <v>70</v>
       </c>
+      <c r="D8">
+        <v>61</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -550,6 +571,9 @@
       <c r="C9">
         <v>70</v>
       </c>
+      <c r="D9">
+        <v>59</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -561,6 +585,9 @@
       <c r="C10">
         <v>58</v>
       </c>
+      <c r="D10">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -572,6 +599,9 @@
       <c r="C11">
         <v>61</v>
       </c>
+      <c r="D11">
+        <v>47</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -583,6 +613,9 @@
       <c r="C12">
         <v>49</v>
       </c>
+      <c r="D12">
+        <v>46</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -594,6 +627,9 @@
       <c r="C13">
         <v>64</v>
       </c>
+      <c r="D13">
+        <v>54</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -604,6 +640,9 @@
       </c>
       <c r="C14">
         <v>65</v>
+      </c>
+      <c r="D14">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>